<commit_message>
regression2 resolvido os problemas de calculo de ci e alguns valores da ANOVA
</commit_message>
<xml_diff>
--- a/exemplos_tutorial_quimica_nova/exemplo1.xlsx
+++ b/exemplos_tutorial_quimica_nova/exemplo1.xlsx
@@ -8,17 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documentos\UFSCar\TCC\playlist23\exemplos_tutorial_quimica_nova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386256AB-58F3-42E7-AAF3-F52D53CE1A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6573E437-6B65-43D1-A8D3-4226A9551FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateCount="32000" iterateDelta="9.9999999999999998E-13"/>
+  <calcPr calcId="181029" iterate="1" iterateCount="32000" iterateDelta="9.9999999999999998E-13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -363,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,8 +401,29 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>2</v>
+      </c>
+      <c r="J1">
+        <v>3</v>
+      </c>
+      <c r="K1">
+        <v>12</v>
+      </c>
+      <c r="L1">
+        <v>13</v>
+      </c>
+      <c r="M1">
+        <v>23</v>
+      </c>
+      <c r="N1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -416,8 +445,36 @@
       <c r="G2">
         <v>178.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>A2</f>
+        <v>-1</v>
+      </c>
+      <c r="I2">
+        <f>C2</f>
+        <v>-1</v>
+      </c>
+      <c r="J2">
+        <f>E2</f>
+        <v>-1</v>
+      </c>
+      <c r="K2">
+        <f>A2*C2</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>A2*E2</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f>C2*E2</f>
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <f>A2*C2*E2</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1</v>
       </c>
@@ -439,8 +496,36 @@
       <c r="G3">
         <v>167.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H12" si="0">A3</f>
+        <v>-1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="1">C3</f>
+        <v>-1</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J12" si="2">E3</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K12" si="3">A3*C3</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L12" si="4">A3*E3</f>
+        <v>-1</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M12" si="5">C3*E3</f>
+        <v>-1</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="6">A3*C3*E3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -462,8 +547,36 @@
       <c r="G4">
         <v>225.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-1</v>
       </c>
@@ -485,8 +598,36 @@
       <c r="G5">
         <v>218.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -508,8 +649,36 @@
       <c r="G6">
         <v>86.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -531,8 +700,36 @@
       <c r="G7">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -554,8 +751,36 @@
       <c r="G8">
         <v>195.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -577,8 +802,36 @@
       <c r="G9">
         <v>189.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -600,8 +853,36 @@
       <c r="G10">
         <v>137.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -623,8 +904,36 @@
       <c r="G11">
         <v>135.69999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -645,6 +954,34 @@
       </c>
       <c r="G12">
         <v>137.80000000000001</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>